<commit_message>
updated templates for inv template
</commit_message>
<xml_diff>
--- a/wikischema/File/Absorption_Emission_Spectroscopy_template.xlsx
+++ b/wikischema/File/Absorption_Emission_Spectroscopy_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kai\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kai\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3C488A7-1B2E-4D4E-A727-1269FD41C4C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640F7DA2-57F4-4597-A69C-BBC478BAA09D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,15 +20,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>Absorber Emitter_inchikey &lt;absorber_emitter&gt;</t>
-  </si>
-  <si>
-    <t>Absorber Emitter_molfile</t>
-  </si>
-  <si>
-    <t>Experiment Type &lt;experiment_type&gt;</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+  <si>
+    <t>Analyte_inchikey &lt;anl&gt;</t>
+  </si>
+  <si>
+    <t>Analyte_molfile</t>
+  </si>
+  <si>
+    <t>Analyte concentration [mM] &lt;anl conc&gt;</t>
+  </si>
+  <si>
+    <t>Solvent A_inchikey &lt;solv&gt;</t>
+  </si>
+  <si>
+    <t>Solvent A_molfile</t>
+  </si>
+  <si>
+    <t>Solvent volume [ml] &lt;solv vol&gt;</t>
+  </si>
+  <si>
+    <t>Additives &lt;additives&gt;</t>
+  </si>
+  <si>
+    <t>Additives concentration [mM] &lt;additives conc&gt;</t>
   </si>
   <si>
     <t>Absorption Max [nm] &lt;absorption_max&gt;</t>
@@ -43,25 +58,52 @@
     <t>Emission Intensity Max [nm] &lt;emission_intensity_max&gt;</t>
   </si>
   <si>
-    <t>Intersection [nm] &lt;intersection&gt;</t>
-  </si>
-  <si>
-    <t>Solvent_inchikey &lt;solvent&gt;</t>
-  </si>
-  <si>
-    <t>Solvent_molfile</t>
-  </si>
-  <si>
-    <t>Solvent concentration [µM] &lt;solvent_conc&gt;</t>
+    <t>Absorption Max 2 [nm] &lt;absorption_max_2&gt;</t>
+  </si>
+  <si>
+    <t>Absorption Intensity Max 2 [nm] &lt;absorption_intensity_max_2&gt;</t>
+  </si>
+  <si>
+    <t>Emission Max 2 [nm] &lt;emission_max_2&gt;</t>
+  </si>
+  <si>
+    <t>Emission Intensity Max 2 [nm] &lt;emission_intensity_max_2&gt;</t>
+  </si>
+  <si>
+    <t>Absorption Max 3 [nm] &lt;absorption_max_3&gt;</t>
+  </si>
+  <si>
+    <t>Absorption Intensity Max 3 [nm] &lt;absorption_intensity_max_3&gt;</t>
+  </si>
+  <si>
+    <t>Emission Max 3 [nm] &lt;emission_max_3&gt;</t>
+  </si>
+  <si>
+    <t>Emission Intensity Max 3 [nm] &lt;emission_intensity_max_3&gt;</t>
+  </si>
+  <si>
+    <t>Interception number &lt;interception_number&gt;</t>
+  </si>
+  <si>
+    <t>Interception [nm] &lt;interception&gt;</t>
+  </si>
+  <si>
+    <t>Additives absorption [nm] &lt;additives_absorption&gt;</t>
+  </si>
+  <si>
+    <t>Intensity Additives absorption [nm] &lt;intensity_absorption&gt;</t>
+  </si>
+  <si>
+    <t>Gas &lt;gas&gt;</t>
   </si>
   <si>
     <t>TemperatureP [°C] &lt;temp&gt;</t>
   </si>
   <si>
-    <t>E0 [eV] &lt;intersection&gt;</t>
-  </si>
-  <si>
-    <t>Absorption Coefficient [L/mol⋅cm] &lt;absorption_coefficient&gt;</t>
+    <t>E0 [eV] &lt;auto-generated-E0&gt;</t>
+  </si>
+  <si>
+    <t>Condition &lt;condition&gt;</t>
   </si>
   <si>
     <t>Details &lt;details&gt;</t>
@@ -417,18 +459,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:AE1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="27" max="27" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -479,6 +522,48 @@
       </c>
       <c r="Q1" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>